<commit_message>
vraie version en ligne
</commit_message>
<xml_diff>
--- a/Logiciel_PEP/mysite/polls/static/polls/template_bv_sylog.xlsx
+++ b/Logiciel_PEP/mysite/polls/static/polls/template_bv_sylog.xlsx
@@ -1428,7 +1428,7 @@
       <c r="H3" s="10" t="n"/>
       <c r="I3" s="74" t="inlineStr">
         <is>
-          <t>14 août 2024</t>
+          <t>18 août 2024</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="G4" s="125" t="inlineStr">
         <is>
-          <t>Antony Feord</t>
+          <t>Edgar Duc</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="G8" s="105" t="inlineStr">
         <is>
-          <t>77420 France</t>
+          <t>67000 France</t>
         </is>
       </c>
     </row>

</xml_diff>